<commit_message>
Adjusted and fixed the column letter to number conversion algorithm
</commit_message>
<xml_diff>
--- a/FPL.xlsx
+++ b/FPL.xlsx
@@ -1453,47 +1453,47 @@
       <c r="T25" s="2" t="n"/>
     </row>
     <row r="26">
-      <c r="B26" s="0" t="inlineStr">
+      <c r="B26" t="inlineStr">
         <is>
           <t>Mohamed Salah</t>
         </is>
       </c>
-      <c r="C26" s="0" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>MID</t>
         </is>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" t="n">
         <v>59</v>
       </c>
     </row>
     <row r="27">
-      <c r="B27" s="0" t="inlineStr">
+      <c r="B27" t="inlineStr">
         <is>
           <t>Ollie Watkins</t>
         </is>
       </c>
-      <c r="C27" s="0" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>FWD</t>
         </is>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" t="n">
         <v>59</v>
       </c>
     </row>
     <row r="28">
-      <c r="B28" s="0" t="inlineStr">
+      <c r="B28" t="inlineStr">
         <is>
           <t>Joachim Andersen</t>
         </is>
       </c>
-      <c r="C28" s="0" t="inlineStr">
+      <c r="C28" t="inlineStr">
         <is>
           <t>DEF</t>
         </is>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28" t="n">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added progress bar and status message
</commit_message>
<xml_diff>
--- a/FPL.xlsx
+++ b/FPL.xlsx
@@ -1453,47 +1453,47 @@
       <c r="T25" s="2" t="n"/>
     </row>
     <row r="26">
-      <c r="B26" t="inlineStr">
+      <c r="B26" s="0" t="inlineStr">
         <is>
           <t>Mohamed Salah</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="C26" s="0" t="inlineStr">
         <is>
           <t>MID</t>
         </is>
       </c>
-      <c r="D26" t="n">
+      <c r="D26" s="0" t="n">
         <v>59</v>
       </c>
     </row>
     <row r="27">
-      <c r="B27" t="inlineStr">
+      <c r="B27" s="0" t="inlineStr">
         <is>
           <t>Ollie Watkins</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C27" s="0" t="inlineStr">
         <is>
           <t>FWD</t>
         </is>
       </c>
-      <c r="D27" t="n">
+      <c r="D27" s="0" t="n">
         <v>59</v>
       </c>
     </row>
     <row r="28">
-      <c r="B28" t="inlineStr">
+      <c r="B28" s="0" t="inlineStr">
         <is>
           <t>Joachim Andersen</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C28" s="0" t="inlineStr">
         <is>
           <t>DEF</t>
         </is>
       </c>
-      <c r="D28" t="n">
+      <c r="D28" s="0" t="n">
         <v>51</v>
       </c>
     </row>

</xml_diff>